<commit_message>
Modifying test data - fixing failure
</commit_message>
<xml_diff>
--- a/resources/testdata/ResellerTests.xlsx
+++ b/resources/testdata/ResellerTests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>Type-2</t>
   </si>
   <si>
-    <t>"English (US)"</t>
-  </si>
-  <si>
     <t>commLang</t>
   </si>
   <si>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>autoTestReseller1</t>
+  </si>
+  <si>
+    <t>English (US)</t>
   </si>
 </sst>
 </file>
@@ -477,7 +477,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -492,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,25 +513,25 @@
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -545,25 +545,25 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
         <v>19</v>
       </c>
-      <c r="I2" t="s">
-        <v>20</v>
-      </c>
       <c r="J2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -575,7 +575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -589,7 +589,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -600,7 +600,7 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Failure fixing - Adding data and steps..
</commit_message>
<xml_diff>
--- a/resources/testdata/ResellerTests.xlsx
+++ b/resources/testdata/ResellerTests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>TCID</t>
   </si>
@@ -97,6 +97,18 @@
   </si>
   <si>
     <t>English (US)</t>
+  </si>
+  <si>
+    <t>userIDMPassword</t>
+  </si>
+  <si>
+    <t>Independent12#</t>
+  </si>
+  <si>
+    <t>resNameSuf</t>
+  </si>
+  <si>
+    <t>&amp; brother's</t>
   </si>
 </sst>
 </file>
@@ -490,10 +502,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,7 +514,7 @@
     <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -533,8 +545,14 @@
       <c r="J1" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -564,6 +582,12 @@
       </c>
       <c r="J2" t="s">
         <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding reseller test & data
</commit_message>
<xml_diff>
--- a/resources/testdata/ResellerTests.xlsx
+++ b/resources/testdata/ResellerTests.xlsx
@@ -8,17 +8,18 @@
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
-    <sheet name="searchResellerID" sheetId="5" r:id="rId2"/>
-    <sheet name="searchResellerVat" sheetId="4" r:id="rId3"/>
-    <sheet name="addReseller" sheetId="2" r:id="rId4"/>
-    <sheet name="searchReseller" sheetId="3" r:id="rId5"/>
+    <sheet name="searchResellerInvalidID" sheetId="6" r:id="rId2"/>
+    <sheet name="searchResellerID" sheetId="5" r:id="rId3"/>
+    <sheet name="searchResellerVat" sheetId="4" r:id="rId4"/>
+    <sheet name="addReseller" sheetId="2" r:id="rId5"/>
+    <sheet name="searchReseller" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="43">
   <si>
     <t>TCID</t>
   </si>
@@ -138,6 +139,15 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>searchResellerInvalidID</t>
+  </si>
+  <si>
+    <t>expected</t>
+  </si>
+  <si>
+    <t>Query returned no results.</t>
   </si>
 </sst>
 </file>
@@ -486,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,6 +552,14 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -549,15 +567,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -573,8 +591,11 @@
       <c r="E1" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -585,10 +606,13 @@
         <v>25</v>
       </c>
       <c r="D2">
-        <v>10003</v>
+        <v>-9444</v>
       </c>
       <c r="E2" t="s">
         <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -617,7 +641,7 @@
         <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>35</v>
@@ -633,11 +657,11 @@
       <c r="C2" t="s">
         <v>25</v>
       </c>
-      <c r="D2" t="s">
-        <v>34</v>
+      <c r="D2">
+        <v>10003</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -646,6 +670,55 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
@@ -778,7 +851,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>

</xml_diff>